<commit_message>
Schedule and syllabus updates
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Week-plan" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="101">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -540,7 +540,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)- [ ] [Basic Data Visualization](</t>
+      <t xml:space="preserve">)
+- [ ] [Basic Data Visualization](</t>
     </r>
     <r>
       <rPr>
@@ -559,7 +560,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)- [ ] [Exploratory Data Analysis](</t>
+      <t xml:space="preserve">)
+- [ ] [Exploratory Data Analysis](</t>
     </r>
     <r>
       <rPr>
@@ -1262,6 +1264,46 @@
   </si>
   <si>
     <t xml:space="preserve">- [ ] Reading Quiz Week 8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [Slides]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../slides/08-graphics.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1545,43 +1587,96 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [Slides]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../slides/10b-debugging.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Homework 9]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../homework/09.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Simulation</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">For Class:
-- [ ] [Simulation](</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/01-simulation.html</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)
+    <t xml:space="preserve">For Class:
+- [ ] [Simulation](https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/01-simulation.html)
 Context: 
 - [Free Wifi with Randomness](https://articles.foletta.org/post/random-wifi-password/)
     - [Numerical Integration](../activities/11-numerical-integration.qmd)
 - [Seductions of Sim - Policy as a Simulation Game](https://www.princeton.edu/~starr/17star.html)
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Reading Quiz Week 11</t>
@@ -1627,6 +1722,109 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">- [ ] [Homework 10](../homework/10.qmd)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">For Class:
+- [ ] [Statistical Simulation](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.youtube.com/watch?v=sTXVNbe8fto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) - ~1h long lecture on statistical model simulation
+- [ ] [The Strange Math That Predicts Almost Anything](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.youtube.com/watch?v=KZeIEiBrT_w</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">) - ~30 minutes, Importance of Monte Carlo Simulation</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- [Slides](../slides/12-simulation-2.qmd)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Homework 11]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../homework/11.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactive Graphics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- [ ] Reading Quiz Week 13</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1653,7 +1851,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">../slides-12-simulation-2.qmd</t>
+      <t xml:space="preserve">../slides/13-interactive-graphics.qmd</t>
     </r>
     <r>
       <rPr>
@@ -1667,10 +1865,44 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Interactive Graphics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- [ ] Reading Quiz Week 13</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Homework 12]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../homework/12.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Lists and Nested Data Structures</t>
@@ -1679,7 +1911,87 @@
     <t xml:space="preserve">- [ ] Reading Quiz Week 14</t>
   </si>
   <si>
-    <t xml:space="preserve">High Performance Computing &amp; Final Part 1</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [Slides]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../slides/14-lists.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Homework 13]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../homework/13.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Part 1</t>
   </si>
   <si>
     <t xml:space="preserve">Final Exam</t>
@@ -1713,15 +2025,6 @@
   </si>
   <si>
     <t xml:space="preserve">Final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">midnight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hwk resub deadline</t>
   </si>
   <si>
     <t xml:space="preserve">Description</t>
@@ -1904,17 +2207,17 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="64.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="101.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="33.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="33.67"/>
@@ -1922,7 +2225,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="45.94"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1951,7 +2254,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="true" ht="59.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="1" customFormat="true" ht="236.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -1980,7 +2283,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="true" ht="251.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="1" customFormat="true" ht="169.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -2009,7 +2312,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="376.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="1" customFormat="true" ht="233.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -2038,7 +2341,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="342.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="245.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
@@ -2067,7 +2370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="422.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="326.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
@@ -2096,7 +2399,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="387.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="259.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
@@ -2125,7 +2428,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="365.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="236.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
@@ -2154,7 +2457,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="331.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="245.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
@@ -2170,12 +2473,20 @@
       <c r="E9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="I9" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -2183,18 +2494,18 @@
         <v>45951</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
       <c r="G10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="502.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="382.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
@@ -2202,22 +2513,28 @@
         <v>45958</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="183.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
@@ -2225,19 +2542,28 @@
         <v>45965</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="71.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
@@ -2245,15 +2571,25 @@
         <v>45972</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="0"/>
+        <v>64</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="G13" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
@@ -2261,15 +2597,26 @@
         <v>45979</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
@@ -2277,11 +2624,23 @@
         <v>45993</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,27 +2651,27 @@
         <v>46000</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="n">
         <v>46008</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" display="https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/01-simulation.html"/>
+    <hyperlink ref="D12" r:id="rId1" display="For Class:&#10;&#10;- [ ] [Simulation](https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/01-simulation.html)&#10;&#10;Context: &#10;&#10;- [Free Wifi with Randomness](https://articles.foletta.org/post/random-wifi-password/)&#10;    - [Numerical Integration](../activities/11-numerical-integration.qmd)&#10;&#10;- [Seductions of Sim - Policy as a Simulation Game](https://www.princeton.edu/~starr/17star.html)&#10;&#10;"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2331,24 +2690,24 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,13 +2715,13 @@
         <v>20251023</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,45 +2729,30 @@
         <v>20251217</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>20251017</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>20251208</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2428,7 +2772,7 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -2439,21 +2783,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>20250825</v>
@@ -2464,7 +2808,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20250901</v>
@@ -2472,7 +2816,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>20251020</v>
@@ -2483,7 +2827,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>20251126</v>
@@ -2494,7 +2838,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>20251215</v>
@@ -2505,10 +2849,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates -- weeks and first day slides
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="101">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -55,7 +55,7 @@
   </si>
   <si>
     <t xml:space="preserve">For Class: 
-- [ ] Read the [syllabus](syllabus.qmd)
+- [ ] Read the [syllabus](../syllabus.qmd)
 - [ ] Read [Computer Basics](https://srvanderplas.github.io/stat-computing-r-python/part-tools/01-computer-basics.html)
 - [ ] Read [Setting up your Computer](https://srvanderplas.github.io/stat-computing-r-python/part-tools/02-setting-up-computer.html)
 - [ ] Read [Rstudio’s Interface](https://srvanderplas.github.io/stat-computing-r-python/part-tools/03-Rstudio-interface.html)
@@ -1466,8 +1466,25 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">)
-- [ ] [Opinionated Analysis Development](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/16973344600006387?auth=SAML) (Recommended)
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Optional)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Opinionated Analysis Development](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/16973344600006387?auth=SAML) (Recommended)
 - How important is long-term reproducibility?  
 - How do the two articles differ with respect to types of reproducibility?   
 - What attempts at reproducibility worked and didn't work in each article?  
@@ -1573,7 +1590,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">../slides/10a-latex-markdown.qmd</t>
+      <t xml:space="preserve">../slides/10a-debugging.qmd</t>
     </r>
     <r>
       <rPr>
@@ -1613,7 +1630,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">../slides/10b-debugging.qmd</t>
+      <t xml:space="preserve">../slides/10b-reproducibility.qmd</t>
     </r>
     <r>
       <rPr>
@@ -1627,59 +1644,52 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- [ ] [Homework 9]</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">../homework/09.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Lists and Nested Data Structures</t>
   </si>
   <si>
-    <t xml:space="preserve">For Class:  
-- [ ] [Functional Programming](https://srvanderplas.github.io/stat-computing-r-python/part-wrangling/08-functional-prog.html) 
-- [ ] [Functional Programming (Advanced R)](http://adv-r.had.co.nz/Functional-programming.html) 
-- [ ] Optional: [Functional Programming HOWTO (Python)](https://docs.python.org/3/howto/functional.html) 
-- [ ] Optional: [Record-based Data and List Processing Strategies](https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/04-xml-json-list-processing.html)     
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">For Class:  
+- [ ] [Functional Programming](https://srvanderplas.github.io/stat-computing-r-python/part-wrangling/08-functional-prog.html)
 More practice with list processing, using JSON and XML files.    
 Context:  
-- [ ] [Why Functional Programming Should Be the Future of Software](https://spectrum.ieee.org/functional-programming) 
-- [ ] [What is a Monad?](https://www.youtube.com/watch?v=t1e8gqXLbsU) 
-- [ ] [Analyzing Data Insights for Titanic](https://angelicatiara.medium.com/analyzing-data-insights-for-titanic-dataset-1-scala-monads-and-functors-in-functional-fb94dc59b422)  </t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- [ ] [Functional Programming (Advanced R)](http://adv-r.had.co.nz/Functional-programming.html) 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Why Functional Programming Should Be the Future of Software](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174391540006387?auth=SAML) 
+- [ ] [What is a Monad?](https://www.youtube.com/watch?v=t1e8gqXLbsU) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+- [ ] Optional: [Functional Programming HOWTO (Python)](https://docs.python.org/3/howto/functional.html) 
+- [ ] Optional: [Record-based Data and List Processing Strategies](https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/04-xml-json-list-processing.html)     </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Reading Quiz Week 14</t>
@@ -1712,46 +1722,6 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">../slides/11-lists.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- [ ] [Homework 10]</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">../homework/10.qmd</t>
     </r>
     <r>
       <rPr>
@@ -1774,10 +1744,132 @@
 - [Free Wifi with Randomness](https://articles.foletta.org/post/random-wifi-password/)
     - [Numerical Integration](../activities/11-numerical-integration.qmd)
 - [Seductions of Sim - Policy as a Simulation Game](https://www.princeton.edu/~starr/17star.html)
+Probability Theory and Monte Carlohttps://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174402200006387?auth=SAML (This uses Excel for computing, which sucks, but it is also a decent explanation of the process)](- [
+- [Input Analysis](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174402200006387?auth=SAML) ) (Optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- [ ] Reading Quiz Week 11</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [Slides]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../slides/12-simulation.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">For Class:  
+- [ ] [Monte Carlo Simulation](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174409750006387?auth=SAML) 
+- [ ] [Probability Theory Shown by Simulation](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174410770006387?auth=SAML) (Optional) 
+- [ ] [Resampling Methods](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174411360006387?auth=SAML) (Optional)  
+Historically, students have a very hard time with the simulation question on the statistics qualifier. I’m experimenting this year with some ways to reinforce this material, despite the fact that you’ll be asked to apply simulation to models and use cases you may not have learned yet, since Stat 850 is taken during your first semester. [This book](https://learning.oreilly.com/library/view/simulation-for-data/9781785881169/?sso_link=yes&amp;sso_link_from=unl-edu) is a good resource for you to keep in mind when studying for the qualifying exam and is available online for free through the library.   
+Other Resources:  
+- [ ] [Statistical Simulation](https://www.youtube.com/watch?v= sTXVNbe8fto) - ~1h long lecture on statistical model simulation 
+- [ ] [The Strange Math That Predicts Almost Anything](https://www.youtube.com/watch?v=KZeIEiBrT_w) - ~30 minutes, Importance of Monte Carlo Simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- [Slides](../slides/12-simulation-2.qmd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanksgiving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enjoy a break!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Class – Thanksgiving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactive Graphics</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">For Class:
+- [ ] [Animated and Interactive Graphics](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/07-intro-interactive-graphics.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
+Context: 
+- [ ] [Reddit thread on professional web app frameworks vs. Shiny](</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.reddit.com/r/rstats/comments/1j0b9mj/as_an_r_shiny_user_seeing_professional_web_apps/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">- [ ] Reading Quiz Week 11</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">- [ ] Reading Quiz Week 13</t>
   </si>
   <si>
     <r>
@@ -1806,7 +1898,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">../slides/12-simulation.qmd</t>
+      <t xml:space="preserve">../slides/13-interactive-graphics.qmd</t>
     </r>
     <r>
       <rPr>
@@ -1820,196 +1912,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">- [ ] [Homework 11](../homework/11.qmd)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">For Class:
-- [ ] [Statistical Simulation](</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.youtube.com/watch?v=sTXVNbe8fto</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">) - ~1h long lecture on statistical model simulation
-- [ ] [The Strange Math That Predicts Almost Anything](</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.youtube.com/watch?v=KZeIEiBrT_w</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">) - ~30 minutes, Importance of Monte Carlo Simulation</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- [Slides](../slides/12-simulation-2.qmd)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- [ ] [Homework 11]</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">../homework/11.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Interactive Graphics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- [ ] Reading Quiz Week 13</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- [Slides]</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">../slides/13-interactive-graphics.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- [ ] [Homework 12]</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">../homework/12.qmd</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Final Part 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Everything!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Final Exam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Everything!</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
@@ -2076,7 +1985,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2119,6 +2028,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2163,7 +2077,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2196,6 +2110,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2220,9 +2142,9 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16:D17"/>
+      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2266,7 +2188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="true" ht="236.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="1" customFormat="true" ht="231.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -2295,7 +2217,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="true" ht="169.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="1" customFormat="true" ht="181.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
@@ -2353,7 +2275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="245.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="248" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
@@ -2517,7 +2439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="382.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="393.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
@@ -2542,11 +2464,8 @@
       <c r="H11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="169.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
@@ -2554,28 +2473,25 @@
         <v>45965</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="24.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="68.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
@@ -2583,28 +2499,25 @@
         <v>45972</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="135.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
@@ -2612,91 +2525,105 @@
         <v>45979</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="24.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="n">
-        <v>45993</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="9" t="n">
+        <v>45986</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="0"/>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="113.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>46000</v>
+        <v>45993</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="0"/>
-      <c r="F16" s="0"/>
-      <c r="G16" s="0"/>
-      <c r="H16" s="0"/>
-      <c r="I16" s="0"/>
+        <v>76</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="n">
+        <v>46000</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="n">
         <v>46008</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
+      <c r="D18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1" display="For Class:&#10;&#10;- [ ] [Simulation](https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/01-simulation.html)&#10;&#10;Context: &#10;&#10;- [Free Wifi with Randomness](https://articles.foletta.org/post/random-wifi-password/)&#10;    - [Numerical Integration](../activities/11-numerical-integration.qmd)&#10;&#10;- [Seductions of Sim - Policy as a Simulation Game](https://www.princeton.edu/~starr/17star.html)&#10;&#10;"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2715,63 +2642,63 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="B16:D17 B19"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>20251023</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>20251217</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="8"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
-      <c r="B5" s="8"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2797,7 +2724,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="1" sqref="B16:D17 F28"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2807,21 +2734,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>20250825</v>
@@ -2832,7 +2759,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20250901</v>
@@ -2840,7 +2767,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>20251020</v>
@@ -2851,7 +2778,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>20251126</v>
@@ -2862,7 +2789,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>20251215</v>
@@ -2873,10 +2800,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
404 page and updated schedule
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -1466,25 +1466,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (Optional)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- [ ] [Opinionated Analysis Development](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/16973344600006387?auth=SAML) (Recommended)
+      <t xml:space="preserve">)  (Optional)
+- [ ] [Opinionated Analysis Development](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/16973344600006387?auth=SAML) (Recommended)
 - How important is long-term reproducibility?  
 - How do the two articles differ with respect to types of reproducibility?   
 - What attempts at reproducibility worked and didn't work in each article?  
@@ -1647,49 +1630,15 @@
     <t xml:space="preserve">Lists and Nested Data Structures</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">For Class:  
+    <t xml:space="preserve">For Class:  
 - [ ] [Functional Programming](https://srvanderplas.github.io/stat-computing-r-python/part-wrangling/08-functional-prog.html)
 More practice with list processing, using JSON and XML files.    
 Context:  
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
 - [ ] [Functional Programming (Advanced R)](http://adv-r.had.co.nz/Functional-programming.html) 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- [ ] [Why Functional Programming Should Be the Future of Software](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174391540006387?auth=SAML) 
-- [ ] [What is a Monad?](https://www.youtube.com/watch?v=t1e8gqXLbsU) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
+- [ ] [Why Functional Programming Should Be the Future of Software](https://unl.alma.exlibrisgroup.com/leganto/public/01UON_LINC/citation/17174391540006387?auth=SAML) 
+- [ ] [What is a Monad?](https://www.youtube.com/watch?v=t1e8gqXLbsU)  
 - [ ] Optional: [Functional Programming HOWTO (Python)](https://docs.python.org/3/howto/functional.html) 
 - [ ] Optional: [Record-based Data and List Processing Strategies](https://srvanderplas.github.io/stat-computing-r-python/part-advanced-topics/04-xml-json-list-processing.html)     </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">- [ ] Reading Quiz Week 14</t>
@@ -1845,26 +1794,15 @@
       </rPr>
       <t xml:space="preserve">)
 Context: 
-- [ ] [Reddit thread on professional web app frameworks vs. Shiny](</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://www.reddit.com/r/rstats/comments/1j0b9mj/as_an_r_shiny_user_seeing_professional_web_apps/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)
+- [The Tiger Mom Tax](https://www.propublica.org/article/asians-nearly-twice-as-likely-to-get-higher-price-from-princeton-review)
+- [Rent Going Up? One Company's Algorithm Could Be Why](https://www.propublica.org/article/yieldstar-rent-increase-realpage-rent)
+- [Racial Discrimination in Face Recognition Technology](https://sitn.hms.harvard.edu/flash/2020/racial-discrimination-in-face-recognition-technology/)
+- [Machine Bias](https://www.propublica.org/article/machine-bias-risk-assessments-in-criminal-sentencing)
+Think about: 
+- When is it ethical to use an algorithm to make decisions?
+- When is it unethical to use an algorithm to make decisions?
+- What conditions need to exist for an algorithm to be trustworthy?
+- How do you, as a statistician, ensure that you understand the biases in your models?
 </t>
     </r>
   </si>
@@ -1985,7 +1923,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2028,11 +1966,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2077,7 +2010,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2110,14 +2043,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2141,10 +2066,10 @@
   </sheetPr>
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2527,7 +2452,7 @@
       <c r="C14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>71</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -2544,26 +2469,25 @@
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="3" t="n">
         <v>45986</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E15" s="0"/>
-      <c r="F15" s="0"/>
-      <c r="G15" s="0" t="s">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>75</v>
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="113.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
@@ -2641,7 +2565,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2665,7 +2589,7 @@
       <c r="A2" s="1" t="n">
         <v>20251023</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2679,7 +2603,7 @@
       <c r="A3" s="1" t="n">
         <v>20251217</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2691,14 +2615,14 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
-      <c r="B5" s="10"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2723,7 +2647,7 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Move ugly stuff and link in to slides
</commit_message>
<xml_diff>
--- a/course-schedule.xlsx
+++ b/course-schedule.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="105">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -1324,6 +1324,46 @@
   </si>
   <si>
     <t xml:space="preserve">Midterm Exam</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">- [ ] [Look at the ugly charts y'all made!]</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">../activities/ugly-graphics.qmd</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Reproducibility &amp; Documents</t>
@@ -2082,7 +2122,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F9" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2358,7 +2398,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="24.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
@@ -2376,6 +2416,9 @@
       <c r="H10" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="I10" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="437.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2385,25 +2428,25 @@
         <v>45958</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2414,22 +2457,22 @@
         <v>45965</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="180.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2440,22 +2483,22 @@
         <v>45972</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="247.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,22 +2509,22 @@
         <v>45979</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,17 +2535,17 @@
         <v>45986</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I15" s="5"/>
     </row>
@@ -2514,22 +2557,22 @@
         <v>45993</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I16" s="5"/>
     </row>
@@ -2541,10 +2584,10 @@
         <v>46000</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -2559,10 +2602,10 @@
         <v>46008</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -2592,16 +2635,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,13 +2652,13 @@
         <v>20251023</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2623,13 +2666,13 @@
         <v>20251217</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2677,21 +2720,21 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>20250825</v>
@@ -2702,7 +2745,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>20250901</v>
@@ -2710,7 +2753,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>20251020</v>
@@ -2721,7 +2764,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>20251126</v>
@@ -2732,7 +2775,7 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>20251215</v>
@@ -2743,10 +2786,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>